<commit_message>
Added project: show case before and after
Both cases in one board
Added symbols
</commit_message>
<xml_diff>
--- a/Mitai - NearField_PCB_Probes/H-Field-Near-Field-Probe/Near H-Filed-Probe/Documents/V1_1/BOM/Bill of Materials-H-field-Near-Field-probe - JLCPCB.xlsx
+++ b/Mitai - NearField_PCB_Probes/H-Field-Near-Field-Probe/Near H-Filed-Probe/Documents/V1_1/BOM/Bill of Materials-H-field-Near-Field-probe - JLCPCB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\EE-PCB-Marketing\Mitai - NearField_PCB_Probes\H-Field-Near-Field-Probe\Near H-Filed-Probe\Documents\V1_1\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4EFF1B-4404-4FEB-9C81-91137466959A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B1658B-C6C5-4219-BD1F-47B0D8437BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
     <t>J2</t>
   </si>
   <si>
-    <t>C914556</t>
+    <t>C1509219</t>
   </si>
 </sst>
 </file>
@@ -155,7 +155,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -173,6 +173,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -558,7 +561,7 @@
       <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>